<commit_message>
new and better code
</commit_message>
<xml_diff>
--- a/SoftPACTesting/bin/resources/data/KDT.xlsx
+++ b/SoftPACTesting/bin/resources/data/KDT.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEFD279-960C-43CF-BD72-60C87DBC265A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22C1E62-E35C-4FF1-BC5E-697C0AF6A796}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4095" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>Keyword</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>{{password}}</t>
+  </si>
+  <si>
+    <t>VERIFYTITLE</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>Register Individual</t>
   </si>
 </sst>
 </file>
@@ -198,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -232,7 +241,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -572,11 +584,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,46 +691,58 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="14" t="s">
+        <v>33</v>
+      </c>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="11" t="s">
-        <v>24</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="E9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="B10" s="11"/>
+      <c r="B10" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="C10" s="11"/>
       <c r="D10" s="12"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -730,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386A8A92-97D3-462F-965E-4B5A1AF37519}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +790,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -940,9 +964,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="6"/>
       <c r="E15" s="1"/>

</xml_diff>